<commit_message>
Named constants for JAS converter
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/data_gen/cybox_genj.xlsx
+++ b/pub-jaen/jaen/data_gen/cybox_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="169">
-  <si>
-    <t>Generated from data\cybox.jaen, Wed Feb 22 08:23:30 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="170">
+  <si>
+    <t>Generated from data\cybox.jaen, Wed Feb 22 16:45:24 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -390,136 +390,139 @@
     <t>CyboxObject</t>
   </si>
   <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Device</t>
+    <t>Address (required)</t>
+  </si>
+  <si>
+    <t>Device (required)</t>
   </si>
   <si>
     <t>DeviceObject (Map)</t>
   </si>
   <si>
-    <t>Disk</t>
+    <t>Disk (required)</t>
   </si>
   <si>
     <t>DiskObject (Record)</t>
   </si>
   <si>
-    <t>Disk_Partition</t>
+    <t>Disk_Partition (required)</t>
   </si>
   <si>
     <t>DiskPartitionObject (Record)</t>
   </si>
   <si>
+    <t>Domain_Name (required)</t>
+  </si>
+  <si>
     <t>DomainNameObject (Record)</t>
   </si>
   <si>
-    <t>Email_Message</t>
+    <t>Email_Message (required)</t>
   </si>
   <si>
     <t>EmailMessageObject (Record)</t>
   </si>
   <si>
-    <t>File</t>
+    <t>File (required)</t>
   </si>
   <si>
     <t>FileObject (Record)</t>
   </si>
   <si>
-    <t>Memory</t>
+    <t>Hostname (required)</t>
+  </si>
+  <si>
+    <t>Memory (required)</t>
   </si>
   <si>
     <t>MemoryObject (Record)</t>
   </si>
   <si>
-    <t>Network_Connection</t>
+    <t>Network_Connection (required)</t>
   </si>
   <si>
     <t>NetworkConnectionObject (Record)</t>
   </si>
   <si>
-    <t>Network_Flow</t>
+    <t>Network_Flow (required)</t>
   </si>
   <si>
     <t>NetworkFlowObject (Record)</t>
   </si>
   <si>
-    <t>Network_Packet</t>
+    <t>Network_Packet (required)</t>
   </si>
   <si>
     <t>NetworkPacketObject (Record)</t>
   </si>
   <si>
-    <t>Network_Subnet</t>
+    <t>Network_Subnet (required)</t>
   </si>
   <si>
     <t>NetworkSubnetObject (Record)</t>
   </si>
   <si>
-    <t>Port</t>
-  </si>
-  <si>
-    <t>Process</t>
+    <t>Port (required)</t>
+  </si>
+  <si>
+    <t>Process (required)</t>
   </si>
   <si>
     <t>ProcessObject (Record)</t>
   </si>
   <si>
-    <t>Product</t>
+    <t>Product (required)</t>
   </si>
   <si>
     <t>ProductObject (Record)</t>
   </si>
   <si>
-    <t>Socket_Address</t>
-  </si>
-  <si>
-    <t>System</t>
+    <t>Socket_Address (required)</t>
+  </si>
+  <si>
+    <t>System (required)</t>
   </si>
   <si>
     <t>SystemObject (Record)</t>
   </si>
   <si>
-    <t>URI</t>
+    <t>URI (required)</t>
   </si>
   <si>
     <t>URIObject (Record)</t>
   </si>
   <si>
-    <t>User_Account</t>
+    <t>User_Account (required)</t>
   </si>
   <si>
     <t>UserAccountObject (Record)</t>
   </si>
   <si>
-    <t>User_Session</t>
+    <t>User_Session (required)</t>
   </si>
   <si>
     <t>UserSessionObject (Record)</t>
   </si>
   <si>
-    <t>Volume</t>
+    <t>Volume (required)</t>
   </si>
   <si>
     <t>VolumeObject (Record)</t>
   </si>
   <si>
-    <t>Windows_Registry_Key</t>
+    <t>Windows_Registry_Key (required)</t>
   </si>
   <si>
     <t>WindowsRegistryKeyObject (Record)</t>
   </si>
   <si>
-    <t>Windows_Service</t>
+    <t>Windows_Service (required)</t>
   </si>
   <si>
     <t>WindowsServiceObject (Record)</t>
   </si>
   <si>
-    <t>X509_Certificate</t>
+    <t>X509_Certificate (required)</t>
   </si>
   <si>
     <t>X509CertificateObject (vocab)</t>
@@ -2303,7 +2306,7 @@
         <v>13</v>
       </c>
       <c r="B185" s="6" t="s">
-        <v>124</v>
+        <v>25</v>
       </c>
       <c r="C185" s="6"/>
       <c r="D185" s="6"/>
@@ -2328,7 +2331,7 @@
         <v>1</v>
       </c>
       <c r="C188" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D188" s="8" t="s">
         <v>77</v>
@@ -2340,10 +2343,10 @@
         <v>2</v>
       </c>
       <c r="C189" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="D189" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="D189" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="E189" s="8"/>
     </row>
@@ -2352,10 +2355,10 @@
         <v>3</v>
       </c>
       <c r="C190" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="D190" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="D190" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="E190" s="8"/>
     </row>
@@ -2364,10 +2367,10 @@
         <v>4</v>
       </c>
       <c r="C191" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D191" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="D191" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="E191" s="8"/>
     </row>
@@ -2376,7 +2379,7 @@
         <v>5</v>
       </c>
       <c r="C192" s="8" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
       <c r="D192" s="8" t="s">
         <v>132</v>
@@ -2412,7 +2415,7 @@
         <v>8</v>
       </c>
       <c r="C195" s="8" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="D195" s="8" t="s">
         <v>79</v>
@@ -2424,10 +2427,10 @@
         <v>9</v>
       </c>
       <c r="C196" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D196" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E196" s="8"/>
     </row>
@@ -2436,10 +2439,10 @@
         <v>10</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D197" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E197" s="8"/>
     </row>
@@ -2448,10 +2451,10 @@
         <v>11</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D198" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E198" s="8"/>
     </row>
@@ -2460,10 +2463,10 @@
         <v>12</v>
       </c>
       <c r="C199" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D199" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E199" s="8"/>
     </row>
@@ -2472,10 +2475,10 @@
         <v>13</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D200" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E200" s="8"/>
     </row>
@@ -2484,7 +2487,7 @@
         <v>14</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D201" s="8" t="s">
         <v>88</v>
@@ -2496,10 +2499,10 @@
         <v>15</v>
       </c>
       <c r="C202" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D202" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E202" s="8"/>
     </row>
@@ -2508,10 +2511,10 @@
         <v>16</v>
       </c>
       <c r="C203" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D203" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E203" s="8"/>
     </row>
@@ -2520,7 +2523,7 @@
         <v>17</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D204" s="8" t="s">
         <v>94</v>
@@ -2532,10 +2535,10 @@
         <v>18</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D205" s="8" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E205" s="8"/>
     </row>
@@ -2544,10 +2547,10 @@
         <v>19</v>
       </c>
       <c r="C206" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D206" s="8" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E206" s="8"/>
     </row>
@@ -2556,10 +2559,10 @@
         <v>20</v>
       </c>
       <c r="C207" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D207" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E207" s="8"/>
     </row>
@@ -2568,10 +2571,10 @@
         <v>21</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D208" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E208" s="8"/>
     </row>
@@ -2580,10 +2583,10 @@
         <v>22</v>
       </c>
       <c r="C209" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D209" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E209" s="8"/>
     </row>
@@ -2592,10 +2595,10 @@
         <v>23</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D210" s="8" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E210" s="8"/>
     </row>
@@ -2604,10 +2607,10 @@
         <v>24</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D211" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E211" s="8"/>
     </row>
@@ -2616,10 +2619,10 @@
         <v>25</v>
       </c>
       <c r="C212" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D212" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E212" s="8"/>
     </row>

</xml_diff>